<commit_message>
correction of error 4107
</commit_message>
<xml_diff>
--- a/src/raw_data/correction of detection .xlsx
+++ b/src/raw_data/correction of detection .xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tjasagrabnar/Desktop/magistrska/customer_data_cleanup/src/raw_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D103CBFC-55A8-E242-9624-FA0B544A57EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAB25E10-168D-5F49-A6D5-49A2F4803255}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1740" yWindow="5800" windowWidth="27240" windowHeight="16440" xr2:uid="{2D99D46F-514D-2B46-BA32-84B5FAB9E921}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="161">
   <si>
     <t>CUSTOMER_ID</t>
   </si>
@@ -938,6 +938,24 @@
   </si>
   <si>
     <t>didnt detect duplicates</t>
+  </si>
+  <si>
+    <t>Šaleška ce. B$</t>
+  </si>
+  <si>
+    <t>should also trigger error 4107, invalid abbr</t>
+  </si>
+  <si>
+    <t>Mariborska cesta  N.H.</t>
+  </si>
+  <si>
+    <t>4102, 4106, 4107</t>
+  </si>
+  <si>
+    <t>shouldnt now trigger 4107</t>
+  </si>
+  <si>
+    <t>these two dont want to work together, correcting one leads to the other one being shit</t>
   </si>
 </sst>
 </file>
@@ -1093,7 +1111,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -1108,6 +1126,9 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
@@ -1447,7 +1468,7 @@
   <dimension ref="A1:G37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A29" sqref="A29:F37"/>
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1780,6 +1801,38 @@
         <v>154</v>
       </c>
     </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A23" s="3">
+        <v>91</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D23" s="10" t="s">
+        <v>160</v>
+      </c>
+      <c r="E23" s="3" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A24" s="3">
+        <v>327</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="D24" s="10"/>
+      <c r="E24" s="3" t="s">
+        <v>159</v>
+      </c>
+    </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>26</v>
@@ -1860,10 +1913,12 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="D15:D17"/>
+    <mergeCell ref="D23:D24"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 

</xml_diff>